<commit_message>
Readded Hierarchy (corrupted file)
</commit_message>
<xml_diff>
--- a/Hierarchy.xlsx
+++ b/Hierarchy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acornstairlifts.sharepoint.com/sites/HRMetrics/Shared Documents/000 - Deployed Programs/001 - ADP to Cascade Integration (USA and CAN)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acornstairlifts.sharepoint.com/sites/HRMetrics/Shared Documents/000 - Deployed Programs/adp-cascade-integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{1336E497-4512-4E44-BCDB-00CB1790D711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{820E6207-E8D7-4F7B-A29F-347B7EF6743C}"/>
   <bookViews>
-    <workbookView xWindow="31110" yWindow="-2745" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{D1049F43-42CB-4463-AE7B-8630605902CA}"/>
+    <workbookView xWindow="1710" yWindow="2205" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{D1049F43-42CB-4463-AE7B-8630605902CA}"/>
   </bookViews>
   <sheets>
     <sheet name="usa Conversion" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,41 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'usa Conversion'!$A$1:$C$36</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="126">
   <si>
+    <t>ADP Code</t>
+  </si>
+  <si>
+    <t>Cascade Code</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
     <t>Human Resources</t>
   </si>
   <si>
@@ -38,6 +66,9 @@
     <t>Executive</t>
   </si>
   <si>
+    <t>Facilities</t>
+  </si>
+  <si>
     <t>Installers</t>
   </si>
   <si>
@@ -47,9 +78,24 @@
     <t>Regional Technical Managers</t>
   </si>
   <si>
+    <t>OPS OTR</t>
+  </si>
+  <si>
+    <t>Operations Admin</t>
+  </si>
+  <si>
+    <t>Service Admin</t>
+  </si>
+  <si>
+    <t>Fleet Admin</t>
+  </si>
+  <si>
     <t>IT</t>
   </si>
   <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
     <t>Logistics</t>
   </si>
   <si>
@@ -59,12 +105,21 @@
     <t>Scheduling</t>
   </si>
   <si>
+    <t>Field Support</t>
+  </si>
+  <si>
     <t>Warehouse - KP</t>
   </si>
   <si>
+    <t>Customer Support</t>
+  </si>
+  <si>
     <t>Training</t>
   </si>
   <si>
+    <t>Permits</t>
+  </si>
+  <si>
     <t>Sales - Admin</t>
   </si>
   <si>
@@ -74,36 +129,6 @@
     <t>Sales - Inside Sales Manager</t>
   </si>
   <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Facilities</t>
-  </si>
-  <si>
-    <t>OPS OTR</t>
-  </si>
-  <si>
-    <t>Operations Admin</t>
-  </si>
-  <si>
-    <t>Service Admin</t>
-  </si>
-  <si>
-    <t>Fleet Admin</t>
-  </si>
-  <si>
-    <t>Digital Marketing</t>
-  </si>
-  <si>
-    <t>Field Support</t>
-  </si>
-  <si>
-    <t>Customer Support</t>
-  </si>
-  <si>
-    <t>Permits</t>
-  </si>
-  <si>
     <t>Sales - Surveyors</t>
   </si>
   <si>
@@ -134,13 +159,22 @@
     <t>Production - OH</t>
   </si>
   <si>
-    <t>ADP Code</t>
-  </si>
-  <si>
-    <t>Cascade Code</t>
-  </si>
-  <si>
-    <t>Department</t>
+    <t>Sales - OH</t>
+  </si>
+  <si>
+    <t>Sales - TX</t>
+  </si>
+  <si>
+    <t>policy</t>
+  </si>
+  <si>
+    <t>earningType</t>
+  </si>
+  <si>
+    <t>narrative</t>
+  </si>
+  <si>
+    <t>cascadeAbsenceId</t>
   </si>
   <si>
     <t>PT-PTO</t>
@@ -149,36 +183,54 @@
     <t>FMLA Paid</t>
   </si>
   <si>
+    <t>9a3bf60e-adeb-4407-81d4-a48a6366c2d5</t>
+  </si>
+  <si>
     <t>PTO</t>
   </si>
   <si>
     <t>Paid Time Off</t>
   </si>
   <si>
+    <t>41b37ab2-6272-4c05-9085-b82d37a2dc46</t>
+  </si>
+  <si>
     <t>SICK</t>
   </si>
   <si>
     <t>Sick</t>
   </si>
   <si>
+    <t>839fa520-6312-48cb-9bc7-6aa11205891d</t>
+  </si>
+  <si>
     <t>UTO</t>
   </si>
   <si>
     <t>Unscheduled Time off</t>
   </si>
   <si>
+    <t>0a1616bd-5466-43a3-acdb-c4c42b32bb6e</t>
+  </si>
+  <si>
     <t>BEREAV</t>
   </si>
   <si>
     <t>Bereavement</t>
   </si>
   <si>
+    <t>3aebdb8e-7cc7-45f1-b72f-804e33530b34</t>
+  </si>
+  <si>
     <t>Floating Holiday</t>
   </si>
   <si>
     <t>PT-PTO-C</t>
   </si>
   <si>
+    <t>FMLA PAID</t>
+  </si>
+  <si>
     <t>PT-PTO-CA-NEW</t>
   </si>
   <si>
@@ -209,36 +261,6 @@
     <t>PTO-C</t>
   </si>
   <si>
-    <t>41b37ab2-6272-4c05-9085-b82d37a2dc46</t>
-  </si>
-  <si>
-    <t>839fa520-6312-48cb-9bc7-6aa11205891d</t>
-  </si>
-  <si>
-    <t>earningType</t>
-  </si>
-  <si>
-    <t>policy</t>
-  </si>
-  <si>
-    <t>narrative</t>
-  </si>
-  <si>
-    <t>cascadeAbsenceId</t>
-  </si>
-  <si>
-    <t>0a1616bd-5466-43a3-acdb-c4c42b32bb6e</t>
-  </si>
-  <si>
-    <t>9a3bf60e-adeb-4407-81d4-a48a6366c2d5</t>
-  </si>
-  <si>
-    <t>3aebdb8e-7cc7-45f1-b72f-804e33530b34</t>
-  </si>
-  <si>
-    <t>FMLA PAID</t>
-  </si>
-  <si>
     <t>job_code</t>
   </si>
   <si>
@@ -278,6 +300,12 @@
     <t>Payroll</t>
   </si>
   <si>
+    <t>PAYROLL</t>
+  </si>
+  <si>
+    <t>Recruiter</t>
+  </si>
+  <si>
     <t>47dfe775-7d16-490d-b669-1d1586c8675f</t>
   </si>
   <si>
@@ -371,40 +399,28 @@
     <t>BC Paid Sick</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>11809094-cfe6-4afd-af16-2629b1e80d49</t>
+  </si>
+  <si>
     <t>Patrick Bethell</t>
   </si>
   <si>
+    <t>36e179b2-9ded-40a8-80f6-9beed7245773</t>
+  </si>
+  <si>
     <t>James Bradley</t>
   </si>
   <si>
+    <t>c75c15c8-80fe-4953-8f50-8da8b5947b5f</t>
+  </si>
+  <si>
     <t>Mark Wheeler</t>
-  </si>
-  <si>
-    <t>11809094-cfe6-4afd-af16-2629b1e80d49</t>
-  </si>
-  <si>
-    <t>36e179b2-9ded-40a8-80f6-9beed7245773</t>
-  </si>
-  <si>
-    <t>c75c15c8-80fe-4953-8f50-8da8b5947b5f</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>PAYROLL</t>
-  </si>
-  <si>
-    <t>Recruiter</t>
-  </si>
-  <si>
-    <t>Sales - OH</t>
-  </si>
-  <si>
-    <t>Sales - TX</t>
   </si>
 </sst>
 </file>
@@ -1303,13 +1319,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1320,7 +1336,7 @@
         <v>151</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1331,7 +1347,7 @@
         <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1342,7 +1358,7 @@
         <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1353,7 +1369,7 @@
         <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1364,7 +1380,7 @@
         <v>414</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1375,7 +1391,7 @@
         <v>361</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1386,7 +1402,7 @@
         <v>362</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1397,7 +1413,7 @@
         <v>360</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1408,7 +1424,7 @@
         <v>390</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1419,7 +1435,7 @@
         <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1430,7 +1446,7 @@
         <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1441,7 +1457,7 @@
         <v>359</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1452,7 +1468,7 @@
         <v>149</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1463,7 +1479,7 @@
         <v>314</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1474,7 +1490,7 @@
         <v>392</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1485,7 +1501,7 @@
         <v>312</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1496,7 +1512,7 @@
         <v>145</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1507,7 +1523,7 @@
         <v>353</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1518,7 +1534,7 @@
         <v>356</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1529,7 +1545,7 @@
         <v>352</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1540,7 +1556,7 @@
         <v>367</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1562,7 +1578,7 @@
         <v>319</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1573,7 +1589,7 @@
         <v>363</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1584,7 +1600,7 @@
         <v>181</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1595,7 +1611,7 @@
         <v>364</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1606,7 +1622,7 @@
         <v>348</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1617,7 +1633,7 @@
         <v>415</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1628,7 +1644,7 @@
         <v>366</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1639,7 +1655,7 @@
         <v>315</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1650,7 +1666,7 @@
         <v>392</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1661,7 +1677,7 @@
         <v>390</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1672,7 +1688,7 @@
         <v>388</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1683,7 +1699,7 @@
         <v>391</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1694,7 +1710,7 @@
         <v>413</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1705,7 +1721,7 @@
         <v>427</v>
       </c>
       <c r="C37" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1716,7 +1732,7 @@
         <v>428</v>
       </c>
       <c r="C38" t="s">
-        <v>125</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1743,478 +1759,478 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
         <v>50</v>
       </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
         <v>51</v>
       </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" t="s">
         <v>52</v>
-      </c>
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2240,13 +2256,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2254,10 +2270,10 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2265,10 +2281,10 @@
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2276,10 +2292,10 @@
         <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2287,10 +2303,10 @@
         <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2298,10 +2314,10 @@
         <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2309,10 +2325,10 @@
         <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2320,10 +2336,10 @@
         <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2331,10 +2347,10 @@
         <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2342,7 +2358,7 @@
         <v>800</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2350,10 +2366,10 @@
         <v>500</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2361,7 +2377,7 @@
         <v>500</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2369,7 +2385,7 @@
         <v>450</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2377,7 +2393,7 @@
         <v>400</v>
       </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2385,7 +2401,7 @@
         <v>300</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2393,7 +2409,7 @@
         <v>200</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2417,114 +2433,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2548,34 +2564,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>